<commit_message>
Add function to add emphasis (NOT FINISHED).
</commit_message>
<xml_diff>
--- a/tools/state_transition_table.xlsx
+++ b/tools/state_transition_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NQF06\source\repos\compare_PDF_as_image\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2D37AF-3AD1-43E9-9824-F2DA5094D68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D14421-5905-4421-AB92-37500106D34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="94">
   <si>
     <t>MainWindow</t>
   </si>
@@ -250,9 +250,6 @@
   <si>
     <t>sldScale</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>txtScale</t>
   </si>
   <si>
     <t>txtScale</t>
@@ -449,6 +446,14 @@
     <rPh sb="13" eb="16">
       <t>カコウゴ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>btnFixEmphasis</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chkEmphasis</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -510,12 +515,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -796,13 +802,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK56"/>
+  <dimension ref="A1:AN62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB56" sqref="AB56"/>
+      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -839,11 +845,13 @@
     <col min="35" max="35" width="8.25" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:40">
       <c r="D1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -944,8 +952,17 @@
       <c r="AK1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="E2" t="s">
         <v>46</v>
       </c>
@@ -1019,201 +1036,210 @@
         <v>47</v>
       </c>
       <c r="AJ2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37">
+        <v>64</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:40">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:40">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AC8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AE8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AF9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AC10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AD11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AC12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC13" t="s">
         <v>81</v>
       </c>
-      <c r="AC13" t="s">
-        <v>82</v>
-      </c>
       <c r="AF13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC15" t="s">
         <v>83</v>
       </c>
-      <c r="AC15" t="s">
-        <v>84</v>
-      </c>
       <c r="AD15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AE15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:40">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:40">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:40">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1221,17 +1247,20 @@
         <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1"/>
       <c r="X22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1239,31 +1268,37 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" t="s">
         <v>69</v>
       </c>
-      <c r="O23" t="s">
-        <v>70</v>
-      </c>
       <c r="R23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1271,17 +1306,17 @@
         <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1"/>
       <c r="V24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1289,16 +1324,16 @@
         <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1306,17 +1341,17 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1"/>
       <c r="V26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1324,16 +1359,16 @@
         <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -1341,17 +1376,20 @@
         <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="1"/>
       <c r="U28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -1359,31 +1397,37 @@
         <v>53</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O29" t="s">
         <v>69</v>
       </c>
-      <c r="O29" t="s">
-        <v>70</v>
-      </c>
       <c r="R29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
@@ -1391,17 +1435,17 @@
         <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1"/>
       <c r="Y30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -1409,16 +1453,16 @@
         <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1426,17 +1470,17 @@
         <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1"/>
       <c r="Y32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1444,16 +1488,16 @@
         <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1461,17 +1505,17 @@
         <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="1"/>
       <c r="Y34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40">
       <c r="A35" s="3" t="s">
         <v>37</v>
       </c>
@@ -1479,16 +1523,16 @@
         <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Z35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1496,17 +1540,20 @@
         <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1"/>
       <c r="U36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1514,31 +1561,37 @@
         <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O37" t="s">
         <v>69</v>
       </c>
-      <c r="O37" t="s">
-        <v>70</v>
-      </c>
       <c r="R37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1546,17 +1599,17 @@
         <v>54</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="1"/>
       <c r="AC38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:40">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1564,16 +1617,16 @@
         <v>54</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1581,17 +1634,17 @@
         <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="1"/>
       <c r="AC40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1599,16 +1652,16 @@
         <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1616,17 +1669,17 @@
         <v>53</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="1"/>
       <c r="AC42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1634,16 +1687,16 @@
         <v>53</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40">
       <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
@@ -1651,17 +1704,17 @@
         <v>53</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="1"/>
       <c r="AC44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40">
       <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
@@ -1669,16 +1722,16 @@
         <v>53</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1686,20 +1739,23 @@
         <v>53</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D46" s="1"/>
       <c r="U46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -1707,42 +1763,48 @@
         <v>53</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O47" t="s">
         <v>69</v>
       </c>
-      <c r="O47" t="s">
-        <v>70</v>
-      </c>
       <c r="R47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40">
       <c r="A48" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:40">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -1750,20 +1812,23 @@
         <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D49" s="1"/>
       <c r="U49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1771,37 +1836,43 @@
         <v>53</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O50" t="s">
         <v>69</v>
       </c>
-      <c r="O50" t="s">
-        <v>70</v>
-      </c>
       <c r="R50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM50" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40">
       <c r="A51" s="3" t="s">
         <v>62</v>
       </c>
@@ -1809,20 +1880,23 @@
         <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="1"/>
       <c r="U51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:32">
+        <v>71</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40">
       <c r="A52" s="3" t="s">
         <v>62</v>
       </c>
@@ -1830,78 +1904,201 @@
         <v>53</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O52" t="s">
         <v>69</v>
       </c>
-      <c r="O52" t="s">
-        <v>70</v>
-      </c>
       <c r="R52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:32">
+        <v>70</v>
+      </c>
+      <c r="AM52" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40">
       <c r="A53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:32" s="4" customFormat="1">
-      <c r="A54" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40">
+      <c r="A54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O54" t="s">
+        <v>69</v>
+      </c>
+      <c r="R54" t="s">
+        <v>69</v>
+      </c>
+      <c r="U54" t="s">
+        <v>71</v>
+      </c>
+      <c r="X54" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40">
+      <c r="A55" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" t="s">
+        <v>68</v>
+      </c>
+      <c r="V55" t="s">
+        <v>70</v>
+      </c>
+      <c r="W55" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40">
+      <c r="A56" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40">
+      <c r="A57" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40">
+      <c r="A58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM58" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40">
+      <c r="A59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:40" s="4" customFormat="1">
+      <c r="A60" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:40">
+      <c r="A61" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="55" spans="1:32">
-      <c r="A55" t="s">
+      <c r="AC61" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:40">
+      <c r="A62" t="s">
         <v>86</v>
       </c>
-      <c r="AC55" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD55" t="s">
+      <c r="AC62" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD62" t="s">
         <v>91</v>
       </c>
-      <c r="AE55" t="s">
+      <c r="AE62" t="s">
         <v>91</v>
       </c>
-      <c r="AF55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:32">
-      <c r="A56" t="s">
+      <c r="AF62" t="s">
         <v>87</v>
-      </c>
-      <c r="AC56" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD56" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE56" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF56" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>